<commit_message>
Added code to compute theoretical opt, added Cifar10 sample
</commit_message>
<xml_diff>
--- a/Experiments/dimensionality_reduction_metrics/results/stress_results.xlsx
+++ b/Experiments/dimensionality_reduction_metrics/results/stress_results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:G56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -473,7 +473,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2023-07-12 14:49:13</t>
+          <t>2023-07-13 13:52:52</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -488,19 +488,19 @@
         <v>10</v>
       </c>
       <c r="E2" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="F2" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G2" t="n">
-        <v>0.7069078809027924</v>
+        <v>0.131710986435798</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2023-07-12 14:49:23</t>
+          <t>2023-07-13 13:53:15</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -512,22 +512,22 @@
         <v>100</v>
       </c>
       <c r="D3" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E3" t="n">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="F3" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="G3" t="n">
-        <v>0.7069071435465243</v>
+        <v>0.1255553160724596</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2023-07-12 14:49:26</t>
+          <t>2023-07-13 13:54:36</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -539,22 +539,22 @@
         <v>100</v>
       </c>
       <c r="D4" t="n">
+        <v>15</v>
+      </c>
+      <c r="E4" t="n">
+        <v>5</v>
+      </c>
+      <c r="F4" t="n">
         <v>10</v>
       </c>
-      <c r="E4" t="n">
-        <v>6</v>
-      </c>
-      <c r="F4" t="n">
-        <v>4</v>
-      </c>
       <c r="G4" t="n">
-        <v>0.7069073787882328</v>
+        <v>0.09917470792777466</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2023-07-12 14:49:27</t>
+          <t>2023-07-13 13:55:33</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -566,22 +566,22 @@
         <v>100</v>
       </c>
       <c r="D5" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E5" t="n">
         <v>5</v>
       </c>
       <c r="F5" t="n">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="G5" t="n">
-        <v>0.7069073834053843</v>
+        <v>0.0790987394204756</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2023-07-12 14:49:32</t>
+          <t>2023-07-13 13:56:09</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -593,22 +593,22 @@
         <v>100</v>
       </c>
       <c r="D6" t="n">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="E6" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="F6" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G6" t="n">
-        <v>0.7069088373657431</v>
+        <v>0.0937789226276013</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2023-07-12 14:49:57</t>
+          <t>2023-07-13 13:56:44</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -620,22 +620,22 @@
         <v>100</v>
       </c>
       <c r="D7" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E7" t="n">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="F7" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G7" t="n">
-        <v>0.7069071943221797</v>
+        <v>0.08006628200456611</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2023-07-12 18:35:14</t>
+          <t>2023-07-13 13:56:57</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -647,22 +647,22 @@
         <v>100</v>
       </c>
       <c r="D8" t="n">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="E8" t="n">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="F8" t="n">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="G8" t="n">
-        <v>0.706906474448729</v>
+        <v>0.08041819610189416</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2023-07-12 18:35:20</t>
+          <t>2023-07-13 13:57:11</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -677,19 +677,19 @@
         <v>15</v>
       </c>
       <c r="E9" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F9" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G9" t="n">
-        <v>0.7069065283199855</v>
+        <v>0.1028280604640996</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2023-07-12 18:35:26</t>
+          <t>2023-07-13 13:57:26</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -701,22 +701,22 @@
         <v>100</v>
       </c>
       <c r="D10" t="n">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="E10" t="n">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="F10" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G10" t="n">
-        <v>0.7069070883359996</v>
+        <v>0.1369895252172157</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2023-07-12 18:35:33</t>
+          <t>2023-07-13 13:57:46</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -731,19 +731,19 @@
         <v>15</v>
       </c>
       <c r="E11" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F11" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="G11" t="n">
-        <v>0.7069062779208405</v>
+        <v>0.1051093794084031</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2023-07-12 18:35:36</t>
+          <t>2023-07-13 13:58:46</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -758,19 +758,19 @@
         <v>15</v>
       </c>
       <c r="E12" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="F12" t="n">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="G12" t="n">
-        <v>0.7069060423847821</v>
+        <v>0.1275881992493849</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2023-07-12 18:35:40</t>
+          <t>2023-07-13 13:59:11</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -782,22 +782,22 @@
         <v>100</v>
       </c>
       <c r="D13" t="n">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="E13" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F13" t="n">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="G13" t="n">
-        <v>0.7069062675108337</v>
+        <v>0.1341005658694305</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2023-07-12 18:35:44</t>
+          <t>2023-07-13 13:59:12</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -812,19 +812,19 @@
         <v>15</v>
       </c>
       <c r="E14" t="n">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="F14" t="n">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="G14" t="n">
-        <v>0.7069062636627111</v>
+        <v>0.1247132514469449</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2023-07-12 18:35:44</t>
+          <t>2023-07-13 13:59:20</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -839,19 +839,19 @@
         <v>15</v>
       </c>
       <c r="E15" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F15" t="n">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="G15" t="n">
-        <v>0.7069071243447935</v>
+        <v>0.1001294776400488</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2023-07-12 18:35:55</t>
+          <t>2023-07-13 13:59:56</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -866,13 +866,1093 @@
         <v>15</v>
       </c>
       <c r="E16" t="n">
+        <v>8</v>
+      </c>
+      <c r="F16" t="n">
+        <v>7</v>
+      </c>
+      <c r="G16" t="n">
+        <v>0.09589098551313752</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>2023-07-13 13:59:57</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Cifar10</t>
+        </is>
+      </c>
+      <c r="C17" t="n">
+        <v>100</v>
+      </c>
+      <c r="D17" t="n">
+        <v>10</v>
+      </c>
+      <c r="E17" t="n">
+        <v>3</v>
+      </c>
+      <c r="F17" t="n">
+        <v>7</v>
+      </c>
+      <c r="G17" t="n">
+        <v>0.1270046512035801</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>2023-07-13 14:00:07</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Cifar10</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>100</v>
+      </c>
+      <c r="D18" t="n">
+        <v>20</v>
+      </c>
+      <c r="E18" t="n">
+        <v>10</v>
+      </c>
+      <c r="F18" t="n">
+        <v>10</v>
+      </c>
+      <c r="G18" t="n">
+        <v>0.07743991242442677</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>2023-07-13 14:00:42</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Cifar10</t>
+        </is>
+      </c>
+      <c r="C19" t="n">
+        <v>100</v>
+      </c>
+      <c r="D19" t="n">
+        <v>20</v>
+      </c>
+      <c r="E19" t="n">
+        <v>2</v>
+      </c>
+      <c r="F19" t="n">
+        <v>18</v>
+      </c>
+      <c r="G19" t="n">
+        <v>0.0885836704756105</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>2023-07-13 14:00:58</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Cifar10</t>
+        </is>
+      </c>
+      <c r="C20" t="n">
+        <v>100</v>
+      </c>
+      <c r="D20" t="n">
+        <v>15</v>
+      </c>
+      <c r="E20" t="n">
+        <v>7</v>
+      </c>
+      <c r="F20" t="n">
+        <v>8</v>
+      </c>
+      <c r="G20" t="n">
+        <v>0.09616628760816602</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>2023-07-13 14:01:42</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Cifar10</t>
+        </is>
+      </c>
+      <c r="C21" t="n">
+        <v>100</v>
+      </c>
+      <c r="D21" t="n">
+        <v>20</v>
+      </c>
+      <c r="E21" t="n">
+        <v>15</v>
+      </c>
+      <c r="F21" t="n">
         <v>5</v>
       </c>
-      <c r="F16" t="n">
+      <c r="G21" t="n">
+        <v>0.09119282752262557</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>2023-07-13 14:01:56</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Cifar10</t>
+        </is>
+      </c>
+      <c r="C22" t="n">
+        <v>100</v>
+      </c>
+      <c r="D22" t="n">
         <v>10</v>
       </c>
-      <c r="G16" t="n">
-        <v>0.7069062790548946</v>
+      <c r="E22" t="n">
+        <v>0</v>
+      </c>
+      <c r="F22" t="n">
+        <v>10</v>
+      </c>
+      <c r="G22" t="n">
+        <v>0.1509859257583799</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>2023-07-13 14:02:18</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Cifar10</t>
+        </is>
+      </c>
+      <c r="C23" t="n">
+        <v>100</v>
+      </c>
+      <c r="D23" t="n">
+        <v>10</v>
+      </c>
+      <c r="E23" t="n">
+        <v>7</v>
+      </c>
+      <c r="F23" t="n">
+        <v>3</v>
+      </c>
+      <c r="G23" t="n">
+        <v>0.1493972278538974</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>2023-07-13 14:02:54</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Cifar10</t>
+        </is>
+      </c>
+      <c r="C24" t="n">
+        <v>100</v>
+      </c>
+      <c r="D24" t="n">
+        <v>20</v>
+      </c>
+      <c r="E24" t="n">
+        <v>8</v>
+      </c>
+      <c r="F24" t="n">
+        <v>12</v>
+      </c>
+      <c r="G24" t="n">
+        <v>0.07698831876516872</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>2023-07-13 14:03:03</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Cifar10</t>
+        </is>
+      </c>
+      <c r="C25" t="n">
+        <v>100</v>
+      </c>
+      <c r="D25" t="n">
+        <v>20</v>
+      </c>
+      <c r="E25" t="n">
+        <v>0</v>
+      </c>
+      <c r="F25" t="n">
+        <v>20</v>
+      </c>
+      <c r="G25" t="n">
+        <v>0.1069799765618515</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>2023-07-13 18:31:17</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Cifar10</t>
+        </is>
+      </c>
+      <c r="C26" t="n">
+        <v>100</v>
+      </c>
+      <c r="D26" t="n">
+        <v>40</v>
+      </c>
+      <c r="E26" t="n">
+        <v>0</v>
+      </c>
+      <c r="F26" t="n">
+        <v>40</v>
+      </c>
+      <c r="G26" t="n">
+        <v>0.07262761178561125</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>2023-07-13 18:32:48</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Cifar10</t>
+        </is>
+      </c>
+      <c r="C27" t="n">
+        <v>100</v>
+      </c>
+      <c r="D27" t="n">
+        <v>40</v>
+      </c>
+      <c r="E27" t="n">
+        <v>20</v>
+      </c>
+      <c r="F27" t="n">
+        <v>20</v>
+      </c>
+      <c r="G27" t="n">
+        <v>0.04193404720192608</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>2023-07-13 18:33:08</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Cifar10</t>
+        </is>
+      </c>
+      <c r="C28" t="n">
+        <v>100</v>
+      </c>
+      <c r="D28" t="n">
+        <v>30</v>
+      </c>
+      <c r="E28" t="n">
+        <v>25</v>
+      </c>
+      <c r="F28" t="n">
+        <v>5</v>
+      </c>
+      <c r="G28" t="n">
+        <v>0.07330091764988445</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>2023-07-13 18:33:22</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Cifar10</t>
+        </is>
+      </c>
+      <c r="C29" t="n">
+        <v>100</v>
+      </c>
+      <c r="D29" t="n">
+        <v>40</v>
+      </c>
+      <c r="E29" t="n">
+        <v>8</v>
+      </c>
+      <c r="F29" t="n">
+        <v>32</v>
+      </c>
+      <c r="G29" t="n">
+        <v>0.04641677631765279</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>2023-07-13 18:33:29</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Cifar10</t>
+        </is>
+      </c>
+      <c r="C30" t="n">
+        <v>100</v>
+      </c>
+      <c r="D30" t="n">
+        <v>100</v>
+      </c>
+      <c r="E30" t="n">
+        <v>80</v>
+      </c>
+      <c r="F30" t="n">
+        <v>20</v>
+      </c>
+      <c r="G30" t="n">
+        <v>0.02037955076092581</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>2023-07-13 18:33:39</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Cifar10</t>
+        </is>
+      </c>
+      <c r="C31" t="n">
+        <v>100</v>
+      </c>
+      <c r="D31" t="n">
+        <v>40</v>
+      </c>
+      <c r="E31" t="n">
+        <v>10</v>
+      </c>
+      <c r="F31" t="n">
+        <v>30</v>
+      </c>
+      <c r="G31" t="n">
+        <v>0.04548731540644776</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>2023-07-13 18:33:44</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Cifar10</t>
+        </is>
+      </c>
+      <c r="C32" t="n">
+        <v>100</v>
+      </c>
+      <c r="D32" t="n">
+        <v>40</v>
+      </c>
+      <c r="E32" t="n">
+        <v>16</v>
+      </c>
+      <c r="F32" t="n">
+        <v>24</v>
+      </c>
+      <c r="G32" t="n">
+        <v>0.0420676223806413</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>2023-07-13 18:33:53</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Cifar10</t>
+        </is>
+      </c>
+      <c r="C33" t="n">
+        <v>100</v>
+      </c>
+      <c r="D33" t="n">
+        <v>100</v>
+      </c>
+      <c r="E33" t="n">
+        <v>60</v>
+      </c>
+      <c r="F33" t="n">
+        <v>40</v>
+      </c>
+      <c r="G33" t="n">
+        <v>0.01717852243545198</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>2023-07-13 18:34:00</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Cifar10</t>
+        </is>
+      </c>
+      <c r="C34" t="n">
+        <v>100</v>
+      </c>
+      <c r="D34" t="n">
+        <v>100</v>
+      </c>
+      <c r="E34" t="n">
+        <v>90</v>
+      </c>
+      <c r="F34" t="n">
+        <v>10</v>
+      </c>
+      <c r="G34" t="n">
+        <v>0.02637786423938624</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>2023-07-13 18:34:08</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Cifar10</t>
+        </is>
+      </c>
+      <c r="C35" t="n">
+        <v>100</v>
+      </c>
+      <c r="D35" t="n">
+        <v>40</v>
+      </c>
+      <c r="E35" t="n">
+        <v>15</v>
+      </c>
+      <c r="F35" t="n">
+        <v>25</v>
+      </c>
+      <c r="G35" t="n">
+        <v>0.04295792226099069</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>2023-07-13 18:34:11</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>Cifar10</t>
+        </is>
+      </c>
+      <c r="C36" t="n">
+        <v>100</v>
+      </c>
+      <c r="D36" t="n">
+        <v>40</v>
+      </c>
+      <c r="E36" t="n">
+        <v>5</v>
+      </c>
+      <c r="F36" t="n">
+        <v>35</v>
+      </c>
+      <c r="G36" t="n">
+        <v>0.05208312899839939</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>2023-07-13 18:34:19</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Cifar10</t>
+        </is>
+      </c>
+      <c r="C37" t="n">
+        <v>100</v>
+      </c>
+      <c r="D37" t="n">
+        <v>100</v>
+      </c>
+      <c r="E37" t="n">
+        <v>20</v>
+      </c>
+      <c r="F37" t="n">
+        <v>80</v>
+      </c>
+      <c r="G37" t="n">
+        <v>0.02143436501937734</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>2023-07-13 18:34:20</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>Cifar10</t>
+        </is>
+      </c>
+      <c r="C38" t="n">
+        <v>100</v>
+      </c>
+      <c r="D38" t="n">
+        <v>40</v>
+      </c>
+      <c r="E38" t="n">
+        <v>4</v>
+      </c>
+      <c r="F38" t="n">
+        <v>36</v>
+      </c>
+      <c r="G38" t="n">
+        <v>0.05396743801228134</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>2023-07-13 18:34:21</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>Cifar10</t>
+        </is>
+      </c>
+      <c r="C39" t="n">
+        <v>100</v>
+      </c>
+      <c r="D39" t="n">
+        <v>30</v>
+      </c>
+      <c r="E39" t="n">
+        <v>27</v>
+      </c>
+      <c r="F39" t="n">
+        <v>3</v>
+      </c>
+      <c r="G39" t="n">
+        <v>0.08845064468365103</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>2023-07-13 18:34:24</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>Cifar10</t>
+        </is>
+      </c>
+      <c r="C40" t="n">
+        <v>100</v>
+      </c>
+      <c r="D40" t="n">
+        <v>100</v>
+      </c>
+      <c r="E40" t="n">
+        <v>70</v>
+      </c>
+      <c r="F40" t="n">
+        <v>30</v>
+      </c>
+      <c r="G40" t="n">
+        <v>0.01810772067186105</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>2023-07-13 18:34:28</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>Cifar10</t>
+        </is>
+      </c>
+      <c r="C41" t="n">
+        <v>100</v>
+      </c>
+      <c r="D41" t="n">
+        <v>30</v>
+      </c>
+      <c r="E41" t="n">
+        <v>20</v>
+      </c>
+      <c r="F41" t="n">
+        <v>10</v>
+      </c>
+      <c r="G41" t="n">
+        <v>0.05799537784936938</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>2023-07-13 18:34:28</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>Cifar10</t>
+        </is>
+      </c>
+      <c r="C42" t="n">
+        <v>100</v>
+      </c>
+      <c r="D42" t="n">
+        <v>40</v>
+      </c>
+      <c r="E42" t="n">
+        <v>35</v>
+      </c>
+      <c r="F42" t="n">
+        <v>5</v>
+      </c>
+      <c r="G42" t="n">
+        <v>0.06259608640546815</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>2023-07-13 18:34:31</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>Cifar10</t>
+        </is>
+      </c>
+      <c r="C43" t="n">
+        <v>100</v>
+      </c>
+      <c r="D43" t="n">
+        <v>30</v>
+      </c>
+      <c r="E43" t="n">
+        <v>18</v>
+      </c>
+      <c r="F43" t="n">
+        <v>12</v>
+      </c>
+      <c r="G43" t="n">
+        <v>0.055646734966607</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>2023-07-13 18:34:35</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>Cifar10</t>
+        </is>
+      </c>
+      <c r="C44" t="n">
+        <v>100</v>
+      </c>
+      <c r="D44" t="n">
+        <v>100</v>
+      </c>
+      <c r="E44" t="n">
+        <v>0</v>
+      </c>
+      <c r="F44" t="n">
+        <v>100</v>
+      </c>
+      <c r="G44" t="n">
+        <v>0.04800258230487552</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>2023-07-13 18:34:35</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>Cifar10</t>
+        </is>
+      </c>
+      <c r="C45" t="n">
+        <v>100</v>
+      </c>
+      <c r="D45" t="n">
+        <v>100</v>
+      </c>
+      <c r="E45" t="n">
+        <v>50</v>
+      </c>
+      <c r="F45" t="n">
+        <v>50</v>
+      </c>
+      <c r="G45" t="n">
+        <v>0.01718939456395096</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>2023-07-13 18:34:37</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>Cifar10</t>
+        </is>
+      </c>
+      <c r="C46" t="n">
+        <v>100</v>
+      </c>
+      <c r="D46" t="n">
+        <v>100</v>
+      </c>
+      <c r="E46" t="n">
+        <v>30</v>
+      </c>
+      <c r="F46" t="n">
+        <v>70</v>
+      </c>
+      <c r="G46" t="n">
+        <v>0.01869339768709955</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>2023-07-13 18:34:41</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>Cifar10</t>
+        </is>
+      </c>
+      <c r="C47" t="n">
+        <v>100</v>
+      </c>
+      <c r="D47" t="n">
+        <v>40</v>
+      </c>
+      <c r="E47" t="n">
+        <v>25</v>
+      </c>
+      <c r="F47" t="n">
+        <v>15</v>
+      </c>
+      <c r="G47" t="n">
+        <v>0.04343767393705848</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>2023-07-13 18:34:42</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>Cifar10</t>
+        </is>
+      </c>
+      <c r="C48" t="n">
+        <v>100</v>
+      </c>
+      <c r="D48" t="n">
+        <v>30</v>
+      </c>
+      <c r="E48" t="n">
+        <v>5</v>
+      </c>
+      <c r="F48" t="n">
+        <v>25</v>
+      </c>
+      <c r="G48" t="n">
+        <v>0.06098560432451892</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>2023-07-13 18:34:43</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>Cifar10</t>
+        </is>
+      </c>
+      <c r="C49" t="n">
+        <v>100</v>
+      </c>
+      <c r="D49" t="n">
+        <v>100</v>
+      </c>
+      <c r="E49" t="n">
+        <v>40</v>
+      </c>
+      <c r="F49" t="n">
+        <v>60</v>
+      </c>
+      <c r="G49" t="n">
+        <v>0.01749645201503272</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>2023-07-13 18:34:53</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>Cifar10</t>
+        </is>
+      </c>
+      <c r="C50" t="n">
+        <v>100</v>
+      </c>
+      <c r="D50" t="n">
+        <v>30</v>
+      </c>
+      <c r="E50" t="n">
+        <v>12</v>
+      </c>
+      <c r="F50" t="n">
+        <v>18</v>
+      </c>
+      <c r="G50" t="n">
+        <v>0.05412327455653342</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>2023-07-13 18:34:55</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>Cifar10</t>
+        </is>
+      </c>
+      <c r="C51" t="n">
+        <v>100</v>
+      </c>
+      <c r="D51" t="n">
+        <v>40</v>
+      </c>
+      <c r="E51" t="n">
+        <v>10</v>
+      </c>
+      <c r="F51" t="n">
+        <v>30</v>
+      </c>
+      <c r="G51" t="n">
+        <v>0.04548731540644776</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>2023-07-13 18:34:56</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>Cifar10</t>
+        </is>
+      </c>
+      <c r="C52" t="n">
+        <v>100</v>
+      </c>
+      <c r="D52" t="n">
+        <v>30</v>
+      </c>
+      <c r="E52" t="n">
+        <v>15</v>
+      </c>
+      <c r="F52" t="n">
+        <v>15</v>
+      </c>
+      <c r="G52" t="n">
+        <v>0.05364538678876786</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>2023-07-13 18:34:57</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>Cifar10</t>
+        </is>
+      </c>
+      <c r="C53" t="n">
+        <v>100</v>
+      </c>
+      <c r="D53" t="n">
+        <v>40</v>
+      </c>
+      <c r="E53" t="n">
+        <v>30</v>
+      </c>
+      <c r="F53" t="n">
+        <v>10</v>
+      </c>
+      <c r="G53" t="n">
+        <v>0.04796402708238161</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>2023-07-13 18:35:03</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>Cifar10</t>
+        </is>
+      </c>
+      <c r="C54" t="n">
+        <v>100</v>
+      </c>
+      <c r="D54" t="n">
+        <v>100</v>
+      </c>
+      <c r="E54" t="n">
+        <v>10</v>
+      </c>
+      <c r="F54" t="n">
+        <v>90</v>
+      </c>
+      <c r="G54" t="n">
+        <v>0.02648948337033227</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>2023-07-13 18:35:03</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>Cifar10</t>
+        </is>
+      </c>
+      <c r="C55" t="n">
+        <v>100</v>
+      </c>
+      <c r="D55" t="n">
+        <v>30</v>
+      </c>
+      <c r="E55" t="n">
+        <v>3</v>
+      </c>
+      <c r="F55" t="n">
+        <v>27</v>
+      </c>
+      <c r="G55" t="n">
+        <v>0.06766615170927688</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>2023-07-13 18:35:03</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>Cifar10</t>
+        </is>
+      </c>
+      <c r="C56" t="n">
+        <v>100</v>
+      </c>
+      <c r="D56" t="n">
+        <v>30</v>
+      </c>
+      <c r="E56" t="n">
+        <v>0</v>
+      </c>
+      <c r="F56" t="n">
+        <v>30</v>
+      </c>
+      <c r="G56" t="n">
+        <v>0.08717679031747595</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added stress plots, stress_bound_vals
</commit_message>
<xml_diff>
--- a/Experiments/dimensionality_reduction_metrics/results/stress_results.xlsx
+++ b/Experiments/dimensionality_reduction_metrics/results/stress_results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G56"/>
+  <dimension ref="A1:G59"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1955,6 +1955,87 @@
         <v>0.08717679031747595</v>
       </c>
     </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>2023-07-13 21:57:32</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>Cifar10</t>
+        </is>
+      </c>
+      <c r="C57" t="n">
+        <v>100</v>
+      </c>
+      <c r="D57" t="n">
+        <v>10</v>
+      </c>
+      <c r="E57" t="n">
+        <v>2</v>
+      </c>
+      <c r="F57" t="n">
+        <v>8</v>
+      </c>
+      <c r="G57" t="n">
+        <v>0.1302874556367354</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>2023-07-13 21:57:41</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>Cifar10</t>
+        </is>
+      </c>
+      <c r="C58" t="n">
+        <v>100</v>
+      </c>
+      <c r="D58" t="n">
+        <v>30</v>
+      </c>
+      <c r="E58" t="n">
+        <v>8</v>
+      </c>
+      <c r="F58" t="n">
+        <v>22</v>
+      </c>
+      <c r="G58" t="n">
+        <v>0.05650222861550116</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>2023-07-13 21:59:47</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>Cifar10</t>
+        </is>
+      </c>
+      <c r="C59" t="n">
+        <v>100</v>
+      </c>
+      <c r="D59" t="n">
+        <v>100</v>
+      </c>
+      <c r="E59" t="n">
+        <v>34</v>
+      </c>
+      <c r="F59" t="n">
+        <v>66</v>
+      </c>
+      <c r="G59" t="n">
+        <v>0.0181339383423586</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>